<commit_message>
Updated the code in the working phase
</commit_message>
<xml_diff>
--- a/mcmaster_excel/18-8_Stainless_Steel_Flanged_Button_Head_Screws.xlsx
+++ b/mcmaster_excel/18-8_Stainless_Steel_Flanged_Button_Head_Screws.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N63"/>
+  <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,221 +434,133 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Lg.</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Threading</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>FlangeDia.</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Head Ht.</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Style</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Size</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Finish</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>TensileStrength, psi</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>SpecificationsMet</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Pkg.Qty.</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr"/>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Pkg.</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>thread_size</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>material_surface</t>
-        </is>
+      <c r="A1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>3/16"</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Fully Threaded</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0.234"</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0.084"</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Hex</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1/16"</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>__</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>70,000</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>ASME B18.3</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>97654A644</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>$9.61</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>4-40</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>18-8 Stainless Steel</t>
-        </is>
-      </c>
+          <t>Drive</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1/4"</t>
+          <t>Lg.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Fully Threaded</t>
+          <t>Threading</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.234"</t>
+          <t>FlangeDia.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.059"</t>
+          <t>Head Ht.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Hex</t>
+          <t>Style</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1/16"</t>
+          <t>Size</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Passivated</t>
+          <t>Finish</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>70,000</t>
+          <t>TensileStrength, psi</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>__</t>
+          <t>SpecificationsMet</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>97654A341</t>
-        </is>
-      </c>
+          <t>Pkg.Qty.</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>6.20</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>4-40</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>18-8 Stainless Steel</t>
-        </is>
-      </c>
+          <t>Pkg.</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3/8"</t>
+          <t>3/16"</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -663,7 +575,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.059"</t>
+          <t>0.084"</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -678,7 +590,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Passivated</t>
+          <t>__</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -688,7 +600,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>__</t>
+          <t>ASME B18.3</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -698,12 +610,12 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>97654A342</t>
+          <t>97654A644</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>6.79</t>
+          <t>$9.61</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -720,7 +632,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>1/4"</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -770,12 +682,12 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>97654A343</t>
+          <t>97654A341</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>7.00</t>
+          <t>6.20</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -792,7 +704,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3/4"</t>
+          <t>3/8"</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -807,7 +719,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.084"</t>
+          <t>0.059"</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -822,7 +734,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>__</t>
+          <t>Passivated</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -832,7 +744,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>ASME B18.3</t>
+          <t>__</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -842,12 +754,12 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>97654A647</t>
+          <t>97654A342</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>11.58</t>
+          <t>6.79</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -864,7 +776,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1/4"</t>
+          <t>1/2"</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -874,12 +786,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.297"</t>
+          <t>0.234"</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.073"</t>
+          <t>0.059"</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -889,7 +801,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>5/64"</t>
+          <t>1/16"</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -914,7 +826,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>97654A344</t>
+          <t>97654A343</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -924,7 +836,7 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>6-32</t>
+          <t>4-40</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -936,7 +848,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3/8"</t>
+          <t>3/4"</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -946,12 +858,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.297"</t>
+          <t>0.234"</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.073"</t>
+          <t>0.084"</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -961,12 +873,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>5/64"</t>
+          <t>1/16"</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Passivated</t>
+          <t>__</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -976,7 +888,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>__</t>
+          <t>ASME B18.3</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -986,17 +898,17 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>97654A345</t>
+          <t>97654A647</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>7.85</t>
+          <t>11.58</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>6-32</t>
+          <t>4-40</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1008,7 +920,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>1/4"</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1058,12 +970,12 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>97654A346</t>
+          <t>97654A344</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>7.57</t>
+          <t>7.00</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1080,7 +992,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3/4"</t>
+          <t>3/8"</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1130,12 +1042,12 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>97654A611</t>
+          <t>97654A345</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>7.12</t>
+          <t>7.85</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1152,7 +1064,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1"</t>
+          <t>1/2"</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1202,12 +1114,12 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>97654A614</t>
+          <t>97654A346</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>8.13</t>
+          <t>7.57</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1224,7 +1136,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1/4"</t>
+          <t>3/4"</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1234,12 +1146,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.359"</t>
+          <t>0.297"</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.087"</t>
+          <t>0.073"</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1249,7 +1161,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>3/32"</t>
+          <t>5/64"</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1269,22 +1181,22 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>97654A102</t>
+          <t>97654A611</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>11.43</t>
+          <t>7.12</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>8-32</t>
+          <t>6-32</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1296,7 +1208,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3/8"</t>
+          <t>1"</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1306,12 +1218,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.359"</t>
+          <t>0.297"</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.087"</t>
+          <t>0.073"</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1321,7 +1233,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>3/32"</t>
+          <t>5/64"</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1341,22 +1253,22 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>97654A347</t>
+          <t>97654A614</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>11.66</t>
+          <t>8.13</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>8-32</t>
+          <t>6-32</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1368,7 +1280,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>1/4"</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1418,12 +1330,12 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>97654A104</t>
+          <t>97654A102</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>11.91</t>
+          <t>11.43</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -1440,7 +1352,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3/4"</t>
+          <t>3/8"</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1490,12 +1402,12 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>97654A348</t>
+          <t>97654A347</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>14.30</t>
+          <t>11.66</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1512,7 +1424,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1"</t>
+          <t>1/2"</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1562,12 +1474,12 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>97654A617</t>
+          <t>97654A104</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>15.48</t>
+          <t>11.91</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1584,7 +1496,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>3/8"</t>
+          <t>3/4"</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1594,12 +1506,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.406"</t>
+          <t>0.359"</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.101"</t>
+          <t>0.087"</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1609,7 +1521,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>1/8"</t>
+          <t>3/32"</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1634,17 +1546,17 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>97654A141</t>
+          <t>97654A348</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>14.48</t>
+          <t>14.30</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>10-24</t>
+          <t>8-32</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -1656,7 +1568,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>1"</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1666,12 +1578,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.406"</t>
+          <t>0.359"</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.101"</t>
+          <t>0.087"</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1681,7 +1593,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>1/8"</t>
+          <t>3/32"</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1706,17 +1618,17 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>97654A142</t>
+          <t>97654A617</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>12.38</t>
+          <t>15.48</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>10-24</t>
+          <t>8-32</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -1728,7 +1640,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5/8"</t>
+          <t>3/8"</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1778,12 +1690,12 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>97654A143</t>
+          <t>97654A141</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>12.86</t>
+          <t>14.48</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -1800,7 +1712,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>3/4"</t>
+          <t>1/2"</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1850,12 +1762,12 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>97654A144</t>
+          <t>97654A142</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>13.27</t>
+          <t>12.38</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -1872,7 +1784,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1"</t>
+          <t>5/8"</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1917,17 +1829,17 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>25</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>97654A349</t>
+          <t>97654A143</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>9.65</t>
+          <t>12.86</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
@@ -1944,7 +1856,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1 1/2"</t>
+          <t>3/4"</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1989,17 +1901,17 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>25</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>97654A350</t>
+          <t>97654A144</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>11.00</t>
+          <t>13.27</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -2016,7 +1928,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1/4"</t>
+          <t>1"</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2031,7 +1943,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.137"</t>
+          <t>0.101"</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2046,7 +1958,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>__</t>
+          <t>Passivated</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2056,7 +1968,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>ASME B18.3</t>
+          <t>__</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2066,17 +1978,17 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>97654A650</t>
+          <t>97654A349</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>9.61</t>
+          <t>9.65</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>10-32</t>
+          <t>10-24</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
@@ -2088,7 +2000,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>3/8"</t>
+          <t>1 1/2"</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2133,22 +2045,22 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>97654A172</t>
+          <t>97654A350</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>12.14</t>
+          <t>11.00</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>10-32</t>
+          <t>10-24</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -2160,7 +2072,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>1/4"</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2175,7 +2087,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.101"</t>
+          <t>0.137"</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -2190,7 +2102,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Passivated</t>
+          <t>__</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -2200,22 +2112,22 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>__</t>
+          <t>ASME B18.3</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>97654A173</t>
+          <t>97654A650</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>12.38</t>
+          <t>9.61</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -2232,7 +2144,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5/8"</t>
+          <t>3/8"</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2282,12 +2194,12 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>97654A174</t>
+          <t>97654A172</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>12.86</t>
+          <t>12.14</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -2304,7 +2216,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>3/4"</t>
+          <t>1/2"</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2354,12 +2266,12 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>97654A175</t>
+          <t>97654A173</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>14.92</t>
+          <t>12.38</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
@@ -2376,7 +2288,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1"</t>
+          <t>5/8"</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2421,17 +2333,17 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>25</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>97654A351</t>
+          <t>97654A174</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>7.74</t>
+          <t>12.86</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -2448,7 +2360,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1 1/2"</t>
+          <t>3/4"</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2493,17 +2405,17 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>25</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>97654A352</t>
+          <t>97654A175</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>8.80</t>
+          <t>14.92</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
@@ -2520,7 +2432,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1/4"</t>
+          <t>1"</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2530,12 +2442,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.563"</t>
+          <t>0.406"</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.178"</t>
+          <t>0.101"</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -2545,12 +2457,12 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>5/32"</t>
+          <t>1/8"</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>__</t>
+          <t>Passivated</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -2560,7 +2472,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>ASME B18.3</t>
+          <t>__</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2570,17 +2482,17 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>97654A653</t>
+          <t>97654A351</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>14.53</t>
+          <t>7.74</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>1/4"-20</t>
+          <t>10-32</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
@@ -2592,7 +2504,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>3/8"</t>
+          <t>1 1/2"</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2602,12 +2514,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0.563"</t>
+          <t>0.406"</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.132"</t>
+          <t>0.101"</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -2617,7 +2529,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>5/32"</t>
+          <t>1/8"</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2637,22 +2549,22 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>97654A261</t>
+          <t>97654A352</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>15.24</t>
+          <t>8.80</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>1/4"-20</t>
+          <t>10-32</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
@@ -2664,7 +2576,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>1/4"</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2679,7 +2591,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.132"</t>
+          <t>0.178"</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -2694,7 +2606,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Passivated</t>
+          <t>__</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -2704,7 +2616,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>__</t>
+          <t>ASME B18.3</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -2714,12 +2626,12 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>97654A262</t>
+          <t>97654A653</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>5.75</t>
+          <t>14.53</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
@@ -2736,7 +2648,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5/8"</t>
+          <t>3/8"</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2781,17 +2693,17 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>25</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>97654A353</t>
+          <t>97654A261</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>8.72</t>
+          <t>15.24</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
@@ -2808,7 +2720,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>3/4"</t>
+          <t>1/2"</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2858,12 +2770,12 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>97654A264</t>
+          <t>97654A262</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>7.90</t>
+          <t>5.75</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
@@ -2880,7 +2792,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>7/8"</t>
+          <t>5/8"</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2930,12 +2842,12 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>97654A354</t>
+          <t>97654A353</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>7.86</t>
+          <t>8.72</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
@@ -2952,7 +2864,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1"</t>
+          <t>3/4"</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3002,12 +2914,12 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>97654A265</t>
+          <t>97654A264</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>10.57</t>
+          <t>7.90</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
@@ -3024,7 +2936,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1 1/4"</t>
+          <t>7/8"</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3069,17 +2981,17 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>97654A620</t>
+          <t>97654A354</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>6.44</t>
+          <t>7.86</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
@@ -3096,7 +3008,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>1 1/2"</t>
+          <t>1"</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3141,17 +3053,17 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>97654A355</t>
+          <t>97654A265</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>8.50</t>
+          <t>10.57</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
@@ -3168,7 +3080,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>1 3/4"</t>
+          <t>1 1/4"</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3218,12 +3130,12 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>97654A623</t>
+          <t>97654A620</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>9.96</t>
+          <t>6.44</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
@@ -3240,7 +3152,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2"</t>
+          <t>1 1/2"</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3290,12 +3202,12 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>97654A356</t>
+          <t>97654A355</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>9.50</t>
+          <t>8.50</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
@@ -3312,7 +3224,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>3"</t>
+          <t>1 3/4"</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3357,17 +3269,17 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>97654A626</t>
+          <t>97654A623</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2.42</t>
+          <t>9.96</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
@@ -3384,7 +3296,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>3 1/2"</t>
+          <t>2"</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3429,17 +3341,17 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>97654A701</t>
+          <t>97654A356</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>15.80</t>
+          <t>9.50</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
@@ -3456,7 +3368,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>3"</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3501,22 +3413,22 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>97654A629</t>
+          <t>97654A626</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>6.82</t>
+          <t>2.42</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>1/4"-28</t>
+          <t>1/4"-20</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
@@ -3528,7 +3440,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>3/4"</t>
+          <t>3 1/2"</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3573,22 +3485,22 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>97654A632</t>
+          <t>97654A701</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>7.29</t>
+          <t>15.80</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>1/4"-28</t>
+          <t>1/4"-20</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -3600,7 +3512,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>1"</t>
+          <t>1/2"</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3650,12 +3562,12 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>97654A635</t>
+          <t>97654A629</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>7.71</t>
+          <t>6.82</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
@@ -3672,7 +3584,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>3/4"</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3682,12 +3594,12 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>0.688"</t>
+          <t>0.563"</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.166"</t>
+          <t>0.132"</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -3697,7 +3609,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>3/16"</t>
+          <t>5/32"</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -3717,22 +3629,22 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>97654A303</t>
+          <t>97654A632</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>9.52</t>
+          <t>7.29</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>5/16"-18</t>
+          <t>1/4"-28</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
@@ -3744,7 +3656,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5/8"</t>
+          <t>1"</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3754,12 +3666,12 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>0.688"</t>
+          <t>0.563"</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.166"</t>
+          <t>0.132"</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -3769,7 +3681,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>3/16"</t>
+          <t>5/32"</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -3789,22 +3701,22 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>97654A304</t>
+          <t>97654A635</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>11.37</t>
+          <t>7.71</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>5/16"-18</t>
+          <t>1/4"-28</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
@@ -3816,7 +3728,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>3/4"</t>
+          <t>1/2"</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -3866,12 +3778,12 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>97654A305</t>
+          <t>97654A303</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>11.54</t>
+          <t>9.52</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
@@ -3888,7 +3800,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>1"</t>
+          <t>5/8"</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -3938,12 +3850,12 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>97654A306</t>
+          <t>97654A304</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>11.72</t>
+          <t>11.37</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
@@ -3960,7 +3872,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>1 1/4"</t>
+          <t>3/4"</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4005,17 +3917,17 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>97654A638</t>
+          <t>97654A305</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>8.61</t>
+          <t>11.54</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
@@ -4032,7 +3944,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1 1/2"</t>
+          <t>1"</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4077,17 +3989,17 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>97654A357</t>
+          <t>97654A306</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2.42</t>
+          <t>11.72</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
@@ -4104,7 +4016,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2"</t>
+          <t>1 1/4"</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4149,17 +4061,17 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>97654A358</t>
+          <t>97654A638</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2.45</t>
+          <t>8.61</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
@@ -4176,7 +4088,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>1 1/2"</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4186,12 +4098,12 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0.813"</t>
+          <t>0.688"</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.268"</t>
+          <t>0.166"</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -4201,12 +4113,12 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>7/32"</t>
+          <t>3/16"</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>__</t>
+          <t>Passivated</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -4216,27 +4128,27 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>ASME B18.3</t>
+          <t>__</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>97654A656</t>
+          <t>97654A357</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>19.18</t>
+          <t>2.42</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>3/8"-16</t>
+          <t>5/16"-18</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
@@ -4248,7 +4160,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>3/4"</t>
+          <t>2"</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4258,12 +4170,12 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>0.813"</t>
+          <t>0.688"</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.199"</t>
+          <t>0.166"</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -4273,7 +4185,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>7/32"</t>
+          <t>3/16"</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -4293,22 +4205,22 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>97654A332</t>
+          <t>97654A358</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>10.62</t>
+          <t>2.45</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>3/8"-16</t>
+          <t>5/16"-18</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
@@ -4320,7 +4232,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>1"</t>
+          <t>1/2"</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4335,7 +4247,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0.199"</t>
+          <t>0.268"</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -4350,7 +4262,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Passivated</t>
+          <t>__</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -4360,22 +4272,22 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>__</t>
+          <t>ASME B18.3</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>97654A333</t>
+          <t>97654A656</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>11.19</t>
+          <t>19.18</t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
@@ -4392,7 +4304,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>1 1/4"</t>
+          <t>3/4"</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4442,12 +4354,12 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>97654A334</t>
+          <t>97654A332</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>13.13</t>
+          <t>10.62</t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
@@ -4464,7 +4376,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1 1/2"</t>
+          <t>1"</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4509,17 +4421,17 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>97654A359</t>
+          <t>97654A333</t>
         </is>
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>3.05</t>
+          <t>11.19</t>
         </is>
       </c>
       <c r="M57" t="inlineStr">
@@ -4536,7 +4448,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2"</t>
+          <t>1 1/4"</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4581,17 +4493,17 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>97654A641</t>
+          <t>97654A334</t>
         </is>
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>3.05</t>
+          <t>13.13</t>
         </is>
       </c>
       <c r="M58" t="inlineStr">
@@ -4608,7 +4520,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>1"</t>
+          <t>1 1/2"</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4618,12 +4530,12 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.156"</t>
+          <t>0.813"</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.265"</t>
+          <t>0.199"</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -4633,7 +4545,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>5/16"</t>
+          <t>7/32"</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -4658,17 +4570,17 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>97654A702</t>
+          <t>97654A359</t>
         </is>
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>8.65</t>
+          <t>3.05</t>
         </is>
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>1/2"-13</t>
+          <t>3/8"-16</t>
         </is>
       </c>
       <c r="N59" t="inlineStr">
@@ -4680,7 +4592,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>1 1/2"</t>
+          <t>2"</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4690,12 +4602,12 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1.156"</t>
+          <t>0.813"</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.265"</t>
+          <t>0.199"</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -4705,7 +4617,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>5/16"</t>
+          <t>7/32"</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -4730,17 +4642,17 @@
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>97654A703</t>
+          <t>97654A641</t>
         </is>
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>9.60</t>
+          <t>3.05</t>
         </is>
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>1/2"-13</t>
+          <t>3/8"-16</t>
         </is>
       </c>
       <c r="N60" t="inlineStr">
@@ -4752,7 +4664,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2"</t>
+          <t>1"</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4802,12 +4714,12 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>97654A704</t>
+          <t>97654A702</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>13.24</t>
+          <t>8.65</t>
         </is>
       </c>
       <c r="M61" t="inlineStr">
@@ -4824,7 +4736,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2 1/2"</t>
+          <t>1 1/2"</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -4874,12 +4786,12 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>97654A360</t>
+          <t>97654A703</t>
         </is>
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>11.10</t>
+          <t>9.60</t>
         </is>
       </c>
       <c r="M62" t="inlineStr">
@@ -4896,70 +4808,214 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
+          <t>2"</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Fully Threaded</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>1.156"</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0.265"</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Hex</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>5/16"</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Passivated</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>70,000</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>__</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>97654A704</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>13.24</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>1/2"-13</t>
+        </is>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>18-8 Stainless Steel</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2 1/2"</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Fully Threaded</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>1.156"</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>0.265"</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Hex</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>5/16"</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Passivated</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>70,000</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>__</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>97654A360</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>11.10</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>1/2"-13</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>18-8 Stainless Steel</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
           <t>3"</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Fully Threaded</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Fully Threaded</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
         <is>
           <t>1.156"</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="D65" t="inlineStr">
         <is>
           <t>0.265"</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>Hex</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Hex</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
         <is>
           <t>5/16"</t>
         </is>
       </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>Passivated</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>70,000</t>
-        </is>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>__</t>
-        </is>
-      </c>
-      <c r="J63" t="inlineStr">
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Passivated</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>70,000</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>__</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="K63" t="inlineStr">
+      <c r="K65" t="inlineStr">
         <is>
           <t>97654A361</t>
         </is>
       </c>
-      <c r="L63" t="inlineStr">
+      <c r="L65" t="inlineStr">
         <is>
           <t>13.34</t>
         </is>
       </c>
-      <c r="M63" t="inlineStr">
+      <c r="M65" t="inlineStr">
         <is>
           <t>1/2"-13</t>
         </is>
       </c>
-      <c r="N63" t="inlineStr">
+      <c r="N65" t="inlineStr">
         <is>
           <t>18-8 Stainless Steel</t>
         </is>

</xml_diff>